<commit_message>
updated knowledge graph with dummy data and emission factors
</commit_message>
<xml_diff>
--- a/Converter/excel_data/file1.xlsx
+++ b/Converter/excel_data/file1.xlsx
@@ -1,23 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\ClimateBowl-KGConverter\Converter\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657A31D0-CDCE-4C61-A991-513859DE5C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9652B3-80D0-460D-8977-682161717770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="2100" windowWidth="29040" windowHeight="15720" xr2:uid="{48BCC63F-876E-47FE-BABB-84EA2D083638}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48BCC63F-876E-47FE-BABB-84EA2D083638}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
   <si>
     <t>Daten Sachbilanz</t>
   </si>
@@ -189,6 +186,24 @@
   </si>
   <si>
     <t>Nichtmetall</t>
+  </si>
+  <si>
+    <t>GaBi EU: Steel finished cold rolled coil (Worldsteel)</t>
+  </si>
+  <si>
+    <t>GaBi EU-28: Electricity Grid Mix</t>
+  </si>
+  <si>
+    <t>GaBi EU-28: Compressed air, 7 bar, high efficiency</t>
+  </si>
+  <si>
+    <t>kg CO2eq./kg</t>
+  </si>
+  <si>
+    <t>kg CO2eq./MJ</t>
+  </si>
+  <si>
+    <t>kg CO2eq./m³</t>
   </si>
 </sst>
 </file>
@@ -383,6 +398,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -398,7 +414,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,173 +429,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="1. Ziel und Untersuchungsrahmen"/>
-      <sheetName val="2. Sachbilanz"/>
-      <sheetName val="3. Wirkungsabschätzung"/>
-      <sheetName val="4. Auswertung"/>
-      <sheetName val="Detail3"/>
-      <sheetName val="Detail2"/>
-      <sheetName val="Detail1"/>
-      <sheetName val="Emissionsfaktoren_EU"/>
-      <sheetName val="Emissionsfaktoren_DE"/>
-      <sheetName val="Bechmarkdatenbank"/>
-      <sheetName val="Berechnungen"/>
-      <sheetName val="Literatur"/>
-      <sheetName val="Notizen"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7">
-        <row r="3">
-          <cell r="A3" t="str">
-            <v>FCR steel coil</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>kg CO2eq./kg</v>
-          </cell>
-          <cell r="C3">
-            <v>2.35</v>
-          </cell>
-          <cell r="D3" t="str">
-            <v>GaBi EU: Steel finished cold rolled coil (Worldsteel)</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4" t="str">
-            <v>Electricity grid mix</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>kg CO2eq./MJ</v>
-          </cell>
-          <cell r="C4">
-            <v>0.10199999999999999</v>
-          </cell>
-          <cell r="D4" t="str">
-            <v>GaBi EU-28: Electricity Grid Mix</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5" t="str">
-            <v>Compressed air, 7 bar</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>kg CO2eq./m³</v>
-          </cell>
-          <cell r="C5">
-            <v>3.5299999999999998E-2</v>
-          </cell>
-          <cell r="D5" t="str">
-            <v>GaBi EU-28: Compressed air, 7 bar, high efficiency</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>Carbon fibre (PAN-based, HT)</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>kg CO2eq./kg</v>
-          </cell>
-          <cell r="C6">
-            <v>27.6</v>
-          </cell>
-          <cell r="D6" t="str">
-            <v>GaBi EU-28: Carbon fiber (CF; PAN-based; HT) - 11</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>HR steel coil</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>kg CO2eq./kg</v>
-          </cell>
-          <cell r="C7">
-            <v>2.08</v>
-          </cell>
-          <cell r="D7" t="str">
-            <v>GaBi EU: Steel hot rolled coil</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>Process water from surface</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>kg CO2eq./kg</v>
-          </cell>
-          <cell r="C8">
-            <v>1.09E-3</v>
-          </cell>
-          <cell r="D8" t="str">
-            <v>GaBi EU-28: Process water from surface water</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>Natural gas mix</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>kg CO2eq./kg</v>
-          </cell>
-          <cell r="C9">
-            <v>0.42699999999999999</v>
-          </cell>
-          <cell r="D9" t="str">
-            <v>Gabi EU-28: Natural gas mix</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>Carbon dioxide emission</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>kg CO2eq./kg</v>
-          </cell>
-          <cell r="C10">
-            <v>1</v>
-          </cell>
-          <cell r="D10" t="str">
-            <v>n.a.</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11" t="str">
-            <v>Diesel mix</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v>kg CO2 eq./l</v>
-          </cell>
-          <cell r="C11">
-            <v>0.27</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>GaBi EU-28: Diesel mix at filling station</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -902,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1574BB61-5A70-4216-8570-DDAB21DD0B70}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,56 +779,56 @@
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="18"/>
     </row>
     <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="18" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="19" t="s">
+      <c r="L3" s="17"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="18" t="s">
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="21"/>
-      <c r="S3" s="17"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="18"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -1082,22 +930,18 @@
         <v>2023</v>
       </c>
       <c r="N5" s="12">
-        <f>VLOOKUP($K5,[1]Emissionsfaktoren_EU!$A$3:$D$1000,3,0)</f>
         <v>2.35</v>
       </c>
-      <c r="O5" s="13" t="str">
-        <f>VLOOKUP($K5,[1]Emissionsfaktoren_EU!$A$3:$D$1000,2,0)</f>
-        <v>kg CO2eq./kg</v>
-      </c>
-      <c r="P5" s="13" t="str">
-        <f>VLOOKUP($K5,[1]Emissionsfaktoren_EU!$A$3:$D$1000,4,0)</f>
-        <v>GaBi EU: Steel finished cold rolled coil (Worldsteel)</v>
+      <c r="O5" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="P5" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="Q5" s="10">
-        <f t="shared" ref="Q5:Q8" si="0">I5*N5</f>
         <v>3.5266249075</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="15" t="s">
         <v>30</v>
       </c>
       <c r="S5" s="14" t="s">
@@ -1145,22 +989,18 @@
         <v>2023</v>
       </c>
       <c r="N6" s="12">
-        <f>VLOOKUP(K6,[1]Emissionsfaktoren_EU!$A$3:$D$1000,3,0)</f>
         <v>0.10199999999999999</v>
       </c>
-      <c r="O6" s="13" t="str">
-        <f>VLOOKUP($K6,[1]Emissionsfaktoren_EU!$A$3:$D$1000,2,0)</f>
-        <v>kg CO2eq./MJ</v>
-      </c>
-      <c r="P6" s="13" t="str">
-        <f>VLOOKUP($K6,[1]Emissionsfaktoren_EU!$A$3:$D$1000,4,0)</f>
-        <v>GaBi EU-28: Electricity Grid Mix</v>
+      <c r="O6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="Q6" s="10">
-        <f t="shared" si="0"/>
-        <v>2.3949344999999993E-2</v>
-      </c>
-      <c r="R6" s="22" t="s">
+        <v>2.3949345E-2</v>
+      </c>
+      <c r="R6" s="15" t="s">
         <v>30</v>
       </c>
       <c r="S6" s="14" t="s">
@@ -1208,22 +1048,18 @@
         <v>2023</v>
       </c>
       <c r="N7" s="12">
-        <f>VLOOKUP(K7,[1]Emissionsfaktoren_EU!$A$3:$D$1000,3,0)</f>
         <v>3.5299999999999998E-2</v>
       </c>
-      <c r="O7" s="13" t="str">
-        <f>VLOOKUP($K7,[1]Emissionsfaktoren_EU!$A$3:$D$1000,2,0)</f>
-        <v>kg CO2eq./m³</v>
-      </c>
-      <c r="P7" s="13" t="str">
-        <f>VLOOKUP($K7,[1]Emissionsfaktoren_EU!$A$3:$D$1000,4,0)</f>
-        <v>GaBi EU-28: Compressed air, 7 bar, high efficiency</v>
+      <c r="O7" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="Q7" s="10">
-        <f t="shared" si="0"/>
         <v>3.5853041569999999E-3</v>
       </c>
-      <c r="R7" s="22" t="s">
+      <c r="R7" s="15" t="s">
         <v>30</v>
       </c>
       <c r="S7" s="14" t="s">
@@ -1271,22 +1107,18 @@
         <v>2023</v>
       </c>
       <c r="N8" s="12">
-        <f>VLOOKUP(K8,[1]Emissionsfaktoren_EU!$A$3:$D$1000,3,0)</f>
         <v>0.10199999999999999</v>
       </c>
-      <c r="O8" s="13" t="str">
-        <f>VLOOKUP($K8,[1]Emissionsfaktoren_EU!$A$3:$D$1000,2,0)</f>
-        <v>kg CO2eq./MJ</v>
-      </c>
-      <c r="P8" s="13" t="str">
-        <f>VLOOKUP($K8,[1]Emissionsfaktoren_EU!$A$3:$D$1000,4,0)</f>
-        <v>GaBi EU-28: Electricity Grid Mix</v>
+      <c r="O8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P8" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="Q8" s="10">
-        <f t="shared" si="0"/>
         <v>0.21338146224000001</v>
       </c>
-      <c r="R8" s="22" t="s">
+      <c r="R8" s="15" t="s">
         <v>30</v>
       </c>
       <c r="S8" s="14" t="s">

</xml_diff>

<commit_message>
updaetd data and added basic info to dropdown
</commit_message>
<xml_diff>
--- a/Converter/excel_data/file1.xlsx
+++ b/Converter/excel_data/file1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\ClimateBowl-KGConverter\Converter\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9652B3-80D0-460D-8977-682161717770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681316BE-A5A1-4A10-A273-92A3FF4DF92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{48BCC63F-876E-47FE-BABB-84EA2D083638}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{48BCC63F-876E-47FE-BABB-84EA2D083638}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="55">
   <si>
     <t>Daten Sachbilanz</t>
   </si>
@@ -101,9 +101,6 @@
     <t>GWP100 nach IPCC</t>
   </si>
   <si>
-    <t>Blechzuschnitt (Stanzen) 1</t>
-  </si>
-  <si>
     <t>Material</t>
   </si>
   <si>
@@ -113,63 +110,24 @@
     <t>Cradle-to-Gate</t>
   </si>
   <si>
-    <t>Produktion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1 FCR Stahlcoil (HCT490X, t=0,5mm) </t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
-    <t>FCR steel coil</t>
-  </si>
-  <si>
-    <t>EU</t>
-  </si>
-  <si>
-    <t>kg CO2 eq.</t>
-  </si>
-  <si>
     <t>Energie</t>
   </si>
   <si>
-    <t>Gate-to-Gate</t>
-  </si>
-  <si>
     <t>elektrische Energie</t>
   </si>
   <si>
-    <t>MJ</t>
-  </si>
-  <si>
     <t>Electricity grid mix</t>
   </si>
   <si>
     <t>Germany</t>
   </si>
   <si>
-    <t>Druckluft</t>
-  </si>
-  <si>
-    <t>m³</t>
-  </si>
-  <si>
-    <t>Compressed air, 7 bar</t>
-  </si>
-  <si>
     <t>W.1</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3.1</t>
-  </si>
-  <si>
-    <t>Oberflächenvorbehandlung (Laserstrukturieren)</t>
-  </si>
-  <si>
     <t>Gruppe Fluss</t>
   </si>
   <si>
@@ -188,22 +146,61 @@
     <t>Nichtmetall</t>
   </si>
   <si>
-    <t>GaBi EU: Steel finished cold rolled coil (Worldsteel)</t>
-  </si>
-  <si>
-    <t>GaBi EU-28: Electricity Grid Mix</t>
-  </si>
-  <si>
-    <t>GaBi EU-28: Compressed air, 7 bar, high efficiency</t>
-  </si>
-  <si>
     <t>kg CO2eq./kg</t>
   </si>
   <si>
-    <t>kg CO2eq./MJ</t>
-  </si>
-  <si>
-    <t>kg CO2eq./m³</t>
+    <t>End-of-Life</t>
+  </si>
+  <si>
+    <t>Entsorgung</t>
+  </si>
+  <si>
+    <t>Gate-to-Grave</t>
+  </si>
+  <si>
+    <t>Entsorgung gebrauchter elektronischer Industriegeräte</t>
+  </si>
+  <si>
+    <t>Treatment of used industrial electronic device, mechanical treatment</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>kg CO2eq.</t>
+  </si>
+  <si>
+    <t>Nutzungsphase</t>
+  </si>
+  <si>
+    <t>Nutzung</t>
+  </si>
+  <si>
+    <t>kWh</t>
+  </si>
+  <si>
+    <t>kg CO2eq./kWh</t>
+  </si>
+  <si>
+    <t>SFM Vormontage</t>
+  </si>
+  <si>
+    <t>Vorkette</t>
+  </si>
+  <si>
+    <t>KB Fuß BG, Rohteil</t>
+  </si>
+  <si>
+    <t>Steel screw</t>
+  </si>
+  <si>
+    <t>KB Fuß BG, Umspritzung</t>
+  </si>
+  <si>
+    <t>PVC</t>
+  </si>
+  <si>
+    <t>dummy_data</t>
   </si>
 </sst>
 </file>
@@ -750,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1574BB61-5A70-4216-8570-DDAB21DD0B70}">
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,7 +777,7 @@
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -883,246 +880,238 @@
         <v>20</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="8">
+        <v>3.12</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="10">
+        <v>15.66</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="L5" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="10">
-        <v>1.5006914499999999</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="M5" s="9">
         <v>2023</v>
       </c>
       <c r="N5" s="12">
-        <v>2.35</v>
+        <v>0.318</v>
       </c>
       <c r="O5" s="13" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q5" s="10">
-        <v>3.5266249075</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="S5" s="14" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>41</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="F6" s="8">
-        <v>2</v>
+        <v>3.11</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="I6" s="10">
-        <v>0.23479749999999996</v>
+        <v>0</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M6" s="9">
         <v>2023</v>
       </c>
       <c r="N6" s="12">
-        <v>0.10199999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="O6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P6" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="P6" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="Q6" s="10">
-        <v>2.3949345E-2</v>
+        <v>0</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="S6" s="14" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="D7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="F7" s="8">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="I7" s="10">
-        <v>0.10156669</v>
+        <v>0.04</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M7" s="9">
         <v>2023</v>
       </c>
       <c r="N7" s="12">
-        <v>3.5299999999999998E-2</v>
+        <v>5.78</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q7" s="10">
-        <v>3.5853041569999999E-3</v>
+        <v>0.25</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="S7" s="14" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>41</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="B8" s="8"/>
       <c r="C8" s="9" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="8">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="I8" s="10">
-        <v>2.0919751200000003</v>
+        <v>0.01</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M8" s="9">
         <v>2023</v>
       </c>
       <c r="N8" s="12">
-        <v>0.10199999999999999</v>
+        <v>2.57</v>
       </c>
       <c r="O8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="P8" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="Q8" s="10">
-        <v>0.21338146224000001</v>
+        <v>0.02</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="S8" s="14" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>